<commit_message>
ci: excel has been validated in request orders
</commit_message>
<xml_diff>
--- a/storage/Template/Excel/Ordenes_solicitudes.xlsx
+++ b/storage/Template/Excel/Ordenes_solicitudes.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sergi\Documents\Projects\prisma\prisma-php\storage\Template\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF25DD5C-6291-4AF4-9352-8A93DEE5D6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9946254-AA05-4643-A610-03A23B5D12A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="ORDENES_SERVICIO" sheetId="1" r:id="rId1"/>
+    <sheet name="ORDENES_SOLICITUD" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -167,6 +167,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -218,14 +221,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>58882</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>892291</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>56285</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>271029</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1128251</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>138207</xdr:rowOff>
     </xdr:to>
@@ -256,8 +259,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17195223" y="56285"/>
-          <a:ext cx="2290329" cy="462922"/>
+          <a:off x="22037791" y="56285"/>
+          <a:ext cx="2283835" cy="462922"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -587,7 +590,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -598,93 +601,87 @@
   <dimension ref="A1:T5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.85546875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="8" max="8" width="30.7109375" customWidth="1"/>
-    <col min="9" max="10" width="31.140625" customWidth="1"/>
-    <col min="11" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="13" width="30.7109375" customWidth="1"/>
+    <col min="3" max="13" width="30.7109375" customWidth="1"/>
     <col min="14" max="14" width="50.7109375" customWidth="1"/>
-    <col min="15" max="15" width="27.7109375" customWidth="1"/>
-    <col min="16" max="16" width="29" customWidth="1"/>
-    <col min="17" max="17" width="38.42578125" customWidth="1"/>
-    <col min="18" max="18" width="24.42578125" customWidth="1"/>
-    <col min="19" max="19" width="28.140625" customWidth="1"/>
-    <col min="20" max="20" width="25.42578125" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" customWidth="1"/>
+    <col min="16" max="16" width="40.85546875" customWidth="1"/>
+    <col min="17" max="17" width="40.7109375" customWidth="1"/>
+    <col min="18" max="20" width="30.7109375" customWidth="1"/>
+    <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
     </row>
     <row r="2" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
     </row>
     <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>

</xml_diff>